<commit_message>
Fixed the thirteenth lab
</commit_message>
<xml_diff>
--- a/labs/Lab_13_python_oop/my_payments_analytics_2023_12_24.xlsx
+++ b/labs/Lab_13_python_oop/my_payments_analytics_2023_12_24.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NEDxZ\web_programming\labs\Lab_13_python_oop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5ACB7C1-440F-4B2D-BE2B-D212938EEBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -316,8 +322,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,7 +340,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -342,25 +348,131 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -398,7 +510,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -432,6 +544,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -466,9 +579,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -641,19 +755,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -661,7 +784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -669,488 +792,511 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="B21" t="s">
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="6">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="B22" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="6">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="B23" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="6">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="B24" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="6">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="B25" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="6">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="B26" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="6">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="B27" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="B28" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="B29" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="B30" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C35" t="s">
+      <c r="B35" s="11"/>
+      <c r="C35" s="11" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
+      <c r="D35" s="12"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="5">
         <v>-49946.96</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="6">
         <v>49989.08</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="5">
         <v>-49953.86</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D37">
-        <v>49988.16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
+      <c r="D37" s="6">
+        <v>49988.160000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="5">
         <v>-49957.53</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="6">
         <v>49987.42</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="5">
         <v>-49968.82</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="6">
         <v>49986.51</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="5">
         <v>-49971.65</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="6">
         <v>49983.56</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="5">
         <v>-49976.47</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="6">
         <v>49975.97</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="5">
         <v>-49981.16</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="6">
         <v>49970.96</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="5">
         <v>-49989.55</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="6">
         <v>49968.05</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="5">
         <v>-49992.37</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D44">
-        <v>49965.76</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" t="s">
+      <c r="D44" s="6">
+        <v>49965.760000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="8">
         <v>-49996.95</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="9">
         <v>49959.97</v>
       </c>
     </row>

</xml_diff>